<commit_message>
lastRow COUnt method worked
</commit_message>
<xml_diff>
--- a/EdisonLogs/gps.xlsx
+++ b/EdisonLogs/gps.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Places</t>
   </si>
@@ -24,13 +24,55 @@
     <t>Coordinates</t>
   </si>
   <si>
-    <t>30.3165° N, 78.0322° E</t>
-  </si>
-  <si>
-    <t>nainital</t>
-  </si>
-  <si>
-    <t>29.3919° N, 79.4542° E</t>
+    <t>PreToria</t>
+  </si>
+  <si>
+    <t>25.7479° S, 28.2293° E</t>
+  </si>
+  <si>
+    <t>TimesTamp</t>
+  </si>
+  <si>
+    <t>astana</t>
+  </si>
+  <si>
+    <t>almaty</t>
+  </si>
+  <si>
+    <t>43.2220° N, 76.8512° E</t>
+  </si>
+  <si>
+    <t>murmask</t>
+  </si>
+  <si>
+    <t>tromso</t>
+  </si>
+  <si>
+    <t>51.1605° N, 71.4704° E</t>
+  </si>
+  <si>
+    <t>naples</t>
+  </si>
+  <si>
+    <t>69.6492° N, 18.9553° E</t>
+  </si>
+  <si>
+    <t>milan</t>
+  </si>
+  <si>
+    <t>belgrade</t>
+  </si>
+  <si>
+    <t>45.4642° N, 9.1900° E</t>
+  </si>
+  <si>
+    <t>kingston</t>
+  </si>
+  <si>
+    <t>44.7866° N, 20.4489° E</t>
+  </si>
+  <si>
+    <t>44.2312° N, 76.4860° W</t>
   </si>
 </sst>
 </file>
@@ -370,32 +412,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.5546875" collapsed="false" bestFit="true"/>
+    <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switcherr method integrated with gpsSearcher
</commit_message>
<xml_diff>
--- a/EdisonLogs/gps.xlsx
+++ b/EdisonLogs/gps.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:T35"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Places</t>
   </si>
@@ -118,6 +119,96 @@
   </si>
   <si>
     <t>60.1699° N, 24.9384° E</t>
+  </si>
+  <si>
+    <t>oslo</t>
+  </si>
+  <si>
+    <t>malmo</t>
+  </si>
+  <si>
+    <t>copenhagen</t>
+  </si>
+  <si>
+    <t>odense</t>
+  </si>
+  <si>
+    <t>kiel</t>
+  </si>
+  <si>
+    <t>rostock</t>
+  </si>
+  <si>
+    <t>59.9139° N, 10.7522° E</t>
+  </si>
+  <si>
+    <t>55.6050° N, 13.0038° E</t>
+  </si>
+  <si>
+    <t>55.6761° N, 12.5683° E</t>
+  </si>
+  <si>
+    <t>55.4038° N, 10.4024° E</t>
+  </si>
+  <si>
+    <t>54.3233° N, 10.1228° E</t>
+  </si>
+  <si>
+    <t>54.0924° N, 12.0991° E</t>
+  </si>
+  <si>
+    <t>Svalbard</t>
+  </si>
+  <si>
+    <t>Tromso</t>
+  </si>
+  <si>
+    <t>77.8750° N, 20.9752° E</t>
+  </si>
+  <si>
+    <t>69.6492° N, 18.9553° E</t>
+  </si>
+  <si>
+    <t>Hannover</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>52.3759° N, 9.7320° E</t>
+  </si>
+  <si>
+    <t>53.5511° N, 9.9937° E</t>
+  </si>
+  <si>
+    <t>51.5074° N, 0.1278° W</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>38.7223° N, 9.1393° W</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>bilbao</t>
+  </si>
+  <si>
+    <t>valencia</t>
+  </si>
+  <si>
+    <t>40.4168° N, 3.7038° W</t>
+  </si>
+  <si>
+    <t>43.2630° N, 2.9350° W</t>
+  </si>
+  <si>
+    <t>39.4699° N, 0.3763° W</t>
   </si>
 </sst>
 </file>
@@ -463,16 +554,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -489,18 +580,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -510,16 +609,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A16"/>
+      <selection activeCell="C22" sqref="C22:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -674,6 +773,193 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
handler for pop up in chrome
</commit_message>
<xml_diff>
--- a/EdisonLogs/gps.xlsx
+++ b/EdisonLogs/gps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:T35"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>Places</t>
   </si>
@@ -209,6 +208,9 @@
   </si>
   <si>
     <t>39.4699° N, 0.3763° W</t>
+  </si>
+  <si>
+    <t>Duren</t>
   </si>
 </sst>
 </file>
@@ -554,16 +556,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -580,26 +582,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -611,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
color change and 200 percent inc
</commit_message>
<xml_diff>
--- a/EdisonLogs/gps.xlsx
+++ b/EdisonLogs/gps.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>Places</t>
   </si>
@@ -214,12 +214,19 @@
   </si>
   <si>
     <t>50.8030° N, 6.4811° E</t>
+  </si>
+  <si>
+    <t>unna</t>
+  </si>
+  <si>
+    <t>51.5333,7.6833</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -562,14 +569,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.859375" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -585,10 +592,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -606,9 +613,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
excel iterator new java file
</commit_message>
<xml_diff>
--- a/EdisonLogs/gps.xlsx
+++ b/EdisonLogs/gps.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
   <si>
     <t>Places</t>
   </si>
@@ -216,10 +216,49 @@
     <t>50.8030° N, 6.4811° E</t>
   </si>
   <si>
-    <t>unna</t>
-  </si>
-  <si>
-    <t>51.5333,7.6833</t>
+    <t>brugge</t>
+  </si>
+  <si>
+    <t>brussels</t>
+  </si>
+  <si>
+    <t>51.2089,3.2242</t>
+  </si>
+  <si>
+    <t>50.9333,6.95</t>
+  </si>
+  <si>
+    <t>50.7333,7.1</t>
+  </si>
+  <si>
+    <t>50.35,7.6</t>
+  </si>
+  <si>
+    <t>50.8504,4.3488</t>
+  </si>
+  <si>
+    <t>dusseldorf</t>
+  </si>
+  <si>
+    <t>gent</t>
+  </si>
+  <si>
+    <t>genk</t>
+  </si>
+  <si>
+    <t>antwerp</t>
+  </si>
+  <si>
+    <t>51.05,3.7167</t>
+  </si>
+  <si>
+    <t>51.2217,6.7762</t>
+  </si>
+  <si>
+    <t>50.965,5.5008</t>
+  </si>
+  <si>
+    <t>51.2199,4.4035</t>
   </si>
 </sst>
 </file>
@@ -566,16 +605,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.859375" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.9609375" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
@@ -595,7 +634,47 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed 300% forthe temp
</commit_message>
<xml_diff>
--- a/EdisonLogs/gps.xlsx
+++ b/EdisonLogs/gps.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Places</t>
   </si>
@@ -253,12 +253,31 @@
   </si>
   <si>
     <t>durban</t>
+  </si>
+  <si>
+    <t>9.01.</t>
+  </si>
+  <si>
+    <t>16.68.</t>
+  </si>
+  <si>
+    <t>16.01.</t>
+  </si>
+  <si>
+    <t>15.93.</t>
+  </si>
+  <si>
+    <t>15.37.</t>
+  </si>
+  <si>
+    <t>23.9.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -606,9 +625,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.859375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +646,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +654,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +662,7 @@
         <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +670,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,7 +678,7 @@
         <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,7 +686,7 @@
         <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,9 +709,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>